<commit_message>
oppdatering av bilde. Husk å endre komma til . hjemme
</commit_message>
<xml_diff>
--- a/Resultater/excel-plot/ny_630Ad6.0.xlsx
+++ b/Resultater/excel-plot/ny_630Ad6.0.xlsx
@@ -304,11 +304,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="118753536"/>
-        <c:axId val="118792960"/>
+        <c:axId val="111745280"/>
+        <c:axId val="111784704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="118753536"/>
+        <c:axId val="111745280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,7 +331,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -348,7 +347,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118792960"/>
+        <c:crossAx val="111784704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -356,7 +355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="118792960"/>
+        <c:axId val="111784704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -380,7 +379,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -404,7 +402,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118753536"/>
+        <c:crossAx val="111745280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -617,11 +615,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119538816"/>
-        <c:axId val="119541120"/>
+        <c:axId val="112002176"/>
+        <c:axId val="112004480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119538816"/>
+        <c:axId val="112002176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -644,7 +642,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -661,7 +658,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119541120"/>
+        <c:crossAx val="112004480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -669,7 +666,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119541120"/>
+        <c:axId val="112004480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -693,7 +690,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -717,7 +713,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119538816"/>
+        <c:crossAx val="112002176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -862,11 +858,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119569792"/>
-        <c:axId val="119637888"/>
+        <c:axId val="112029056"/>
+        <c:axId val="112097152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119569792"/>
+        <c:axId val="112029056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -889,7 +885,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -906,7 +901,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119637888"/>
+        <c:crossAx val="112097152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -914,7 +909,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119637888"/>
+        <c:axId val="112097152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -938,7 +933,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -962,7 +956,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119569792"/>
+        <c:crossAx val="112029056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -1108,11 +1102,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119650176"/>
-        <c:axId val="119665024"/>
+        <c:axId val="112125824"/>
+        <c:axId val="112136576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119650176"/>
+        <c:axId val="112125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1135,7 +1129,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1152,7 +1145,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119665024"/>
+        <c:crossAx val="112136576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1160,7 +1153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119665024"/>
+        <c:axId val="112136576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1184,7 +1177,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1208,7 +1200,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119650176"/>
+        <c:crossAx val="112125824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,11 +1413,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119962240"/>
-        <c:axId val="119972992"/>
+        <c:axId val="112167168"/>
+        <c:axId val="112177920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119962240"/>
+        <c:axId val="112167168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1440,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1465,7 +1456,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119972992"/>
+        <c:crossAx val="112177920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1473,7 +1464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119972992"/>
+        <c:axId val="112177920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1497,7 +1488,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1521,7 +1511,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119962240"/>
+        <c:crossAx val="112167168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1666,11 +1656,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121426688"/>
-        <c:axId val="121428992"/>
+        <c:axId val="115532544"/>
+        <c:axId val="115534848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121426688"/>
+        <c:axId val="115532544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1683,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1710,7 +1699,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121428992"/>
+        <c:crossAx val="115534848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1718,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121428992"/>
+        <c:axId val="115534848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1742,7 +1731,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1766,7 +1754,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121426688"/>
+        <c:crossAx val="115532544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1984,11 +1972,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121439744"/>
-        <c:axId val="121466880"/>
+        <c:axId val="115547520"/>
+        <c:axId val="115570560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121439744"/>
+        <c:axId val="115547520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,7 +1999,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2028,7 +2015,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121466880"/>
+        <c:crossAx val="115570560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2036,7 +2023,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121466880"/>
+        <c:axId val="115570560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2060,7 +2047,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2084,7 +2070,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121439744"/>
+        <c:crossAx val="115547520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2182,10 +2168,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>comp!$B$3:$B$10</c:f>
+              <c:f>comp!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.15</c:v>
                 </c:pt>
@@ -2205,9 +2191,15 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
@@ -2256,29 +2248,29 @@
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln>
+              <a:ln w="12700">
                 <a:solidFill>
-                  <a:schemeClr val="accent3"/>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>comp!$D$3:$D$10</c:f>
+              <c:f>comp!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2315,10 +2307,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>comp!$E$3:$E$10</c:f>
+              <c:f>comp!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -2365,10 +2357,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>comp!$F$3:$F$10</c:f>
+              <c:f>comp!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2396,11 +2388,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="121506048"/>
-        <c:axId val="121512704"/>
+        <c:axId val="115941760"/>
+        <c:axId val="115944064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="121506048"/>
+        <c:axId val="115941760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2440,7 +2432,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121512704"/>
+        <c:crossAx val="115944064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2448,7 +2440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="121512704"/>
+        <c:axId val="115944064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="110"/>
@@ -2496,7 +2488,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121506048"/>
+        <c:crossAx val="115941760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="10"/>
@@ -2781,15 +2773,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>638174</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>628649</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6406,10 +6398,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6505,17 +6497,27 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>0.5</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>0.6</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>100</v>
       </c>
     </row>

</xml_diff>